<commit_message>
introduce the vg pack 1.7
</commit_message>
<xml_diff>
--- a/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
+++ b/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_pub\docs\VEEPortingGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4656DD8-2D0A-4437-BDD2-A872760A7190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC6B09-22D2-4673-9622-B97394F04EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="502" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="94">
   <si>
     <t>pack ui</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>10.0.0</t>
+  </si>
+  <si>
+    <t>1.7.0</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1114,9 @@
         <v>92</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="H14" s="10"/>
+      <c r="H14" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="11" t="s">
         <v>7</v>
@@ -1297,13 +1302,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E750B59-6D36-4DC3-86F9-7C4DB63A361C}">
-  <dimension ref="A1:AS179"/>
+  <dimension ref="A1:AS181"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="12" ySplit="3" topLeftCell="M157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H180" sqref="H180"/>
+      <selection pane="bottomRight" activeCell="I181" sqref="I181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18334,67 +18339,67 @@
         <v/>
       </c>
       <c r="AC133" s="1" t="str">
-        <f t="shared" ref="AC133:AC179" si="65">IF($I133=0,"",$G133)</f>
+        <f t="shared" ref="AC133:AC181" si="65">IF($I133=0,"",$G133)</f>
         <v>1.4.0</v>
       </c>
       <c r="AD133" s="1" t="str">
-        <f t="shared" ref="AD133:AD179" si="66">IF($I133=0,"",$A133)</f>
+        <f t="shared" ref="AD133:AD181" si="66">IF($I133=0,"",$A133)</f>
         <v>13.7.2</v>
       </c>
       <c r="AE133" s="1" t="str">
-        <f t="shared" ref="AE133:AE179" si="67">IF($I133=0,"",$I133)</f>
+        <f t="shared" ref="AE133:AE181" si="67">IF($I133=0,"",$I133)</f>
         <v>6.0.0</v>
       </c>
       <c r="AF133" s="1" t="str">
-        <f t="shared" ref="AF133:AF179" si="68">IF($I133=0,"",$D133)</f>
+        <f t="shared" ref="AF133:AF181" si="68">IF($I133=0,"",$D133)</f>
         <v>7.2.0</v>
       </c>
       <c r="AG133" s="1" t="str">
-        <f t="shared" ref="AG133:AG179" si="69">IF($I133=0,"",$H133)</f>
+        <f t="shared" ref="AG133:AG181" si="69">IF($I133=0,"",$H133)</f>
         <v>3.0.1</v>
       </c>
       <c r="AH133" s="1" t="str">
-        <f t="shared" ref="AH133:AH179" si="70">IF($I133=0,"",$B133)</f>
+        <f t="shared" ref="AH133:AH181" si="70">IF($I133=0,"",$B133)</f>
         <v>3.1.0</v>
       </c>
       <c r="AI133" s="1" t="str">
-        <f t="shared" ref="AI133:AI179" si="71">IF($I133=0,"",$K133)</f>
+        <f t="shared" ref="AI133:AI181" si="71">IF($I133=0,"",$K133)</f>
         <v>2.0.2</v>
       </c>
       <c r="AJ133" s="1" t="str">
-        <f t="shared" ref="AJ133:AJ179" si="72">IF($I133=0,"",$L133)</f>
+        <f t="shared" ref="AJ133:AJ181" si="72">IF($I133=0,"",$L133)</f>
         <v>1.0.2</v>
       </c>
       <c r="AL133" s="1" t="str">
-        <f t="shared" ref="AL133:AL179" si="73">IF($J133=0,"",$G133)</f>
+        <f t="shared" ref="AL133:AL181" si="73">IF($J133=0,"",$G133)</f>
         <v/>
       </c>
       <c r="AM133" s="1" t="str">
-        <f t="shared" ref="AM133:AM179" si="74">IF($J133=0,"",$A133)</f>
+        <f t="shared" ref="AM133:AM181" si="74">IF($J133=0,"",$A133)</f>
         <v/>
       </c>
       <c r="AN133" s="1" t="str">
-        <f t="shared" ref="AN133:AN179" si="75">IF($J133=0,"",$J133)</f>
+        <f t="shared" ref="AN133:AN181" si="75">IF($J133=0,"",$J133)</f>
         <v/>
       </c>
       <c r="AO133" s="1" t="str">
-        <f t="shared" ref="AO133:AO179" si="76">IF($J133=0,"",$E133)</f>
+        <f t="shared" ref="AO133:AO181" si="76">IF($J133=0,"",$E133)</f>
         <v/>
       </c>
       <c r="AP133" s="1" t="str">
-        <f t="shared" ref="AP133:AP179" si="77">IF($J133=0,"",$H133)</f>
+        <f t="shared" ref="AP133:AP181" si="77">IF($J133=0,"",$H133)</f>
         <v/>
       </c>
       <c r="AQ133" s="1" t="str">
-        <f t="shared" ref="AQ133:AQ179" si="78">IF($J133=0,"",$B133)</f>
+        <f t="shared" ref="AQ133:AQ181" si="78">IF($J133=0,"",$B133)</f>
         <v/>
       </c>
       <c r="AR133" s="1" t="str">
-        <f t="shared" ref="AR133:AR179" si="79">IF($J133=0,"",$K133)</f>
+        <f t="shared" ref="AR133:AR181" si="79">IF($J133=0,"",$K133)</f>
         <v/>
       </c>
       <c r="AS133" s="1" t="str">
-        <f t="shared" ref="AS133:AS179" si="80">IF($J133=0,"",$L133)</f>
+        <f t="shared" ref="AS133:AS181" si="80">IF($J133=0,"",$L133)</f>
         <v/>
       </c>
     </row>
@@ -23545,7 +23550,7 @@
         <v>14.1.0</v>
       </c>
       <c r="B173" s="3" t="str">
-        <f t="shared" ref="B173:B179" si="128">A173</f>
+        <f t="shared" ref="B173:B181" si="128">A173</f>
         <v>14.1.0</v>
       </c>
       <c r="C173" s="3" t="s">
@@ -24359,21 +24364,21 @@
         <v>14.1.0</v>
       </c>
       <c r="C179" s="3"/>
-      <c r="D179" s="12"/>
-      <c r="E179" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="D179" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E179" s="12"/>
       <c r="F179" s="12"/>
       <c r="G179" s="12" t="s">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="H179" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I179" s="12"/>
-      <c r="J179" s="12" t="s">
-        <v>49</v>
-      </c>
+      <c r="I179" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J179" s="12"/>
       <c r="K179" s="12" t="s">
         <v>29</v>
       </c>
@@ -24381,110 +24386,390 @@
         <v>49</v>
       </c>
       <c r="N179" s="1" t="str">
-        <f t="shared" si="117"/>
+        <f t="shared" ref="N179" si="131">A179</f>
         <v>14.1.0</v>
       </c>
       <c r="O179" s="1" t="str">
-        <f t="shared" si="118"/>
+        <f t="shared" ref="O179" si="132">B179</f>
         <v>14.1.0</v>
       </c>
       <c r="Q179" s="1" t="str">
-        <f t="shared" si="119"/>
+        <f t="shared" ref="Q179" si="133">IF(C179=0,"",$A179)</f>
         <v/>
       </c>
       <c r="R179" s="1" t="str">
-        <f t="shared" si="120"/>
+        <f t="shared" ref="R179" si="134">IF(C179=0,"",$C179)</f>
         <v/>
       </c>
       <c r="S179" s="1" t="str">
-        <f t="shared" si="121"/>
+        <f t="shared" ref="S179" si="135">IF(C179=0,"",$B179)</f>
         <v/>
       </c>
       <c r="U179" s="1" t="str">
-        <f t="shared" si="122"/>
-        <v/>
+        <f t="shared" ref="U179" si="136">IF(D179=0,"",$A179)</f>
+        <v>14.1.0</v>
       </c>
       <c r="V179" s="1" t="str">
-        <f t="shared" si="123"/>
-        <v/>
+        <f t="shared" ref="V179" si="137">IF(D179=0,"",$D179)</f>
+        <v>10.0.0</v>
       </c>
       <c r="W179" s="1" t="str">
-        <f t="shared" si="124"/>
-        <v/>
+        <f t="shared" ref="W179" si="138">IF(D179=0,"",$B179)</f>
+        <v>14.1.0</v>
       </c>
       <c r="Y179" s="1" t="str">
-        <f t="shared" si="125"/>
-        <v>14.1.0</v>
+        <f t="shared" ref="Y179" si="139">IF(E179=0,"",$A179)</f>
+        <v/>
       </c>
       <c r="Z179" s="1" t="str">
-        <f t="shared" si="126"/>
-        <v>4.0.0</v>
+        <f t="shared" ref="Z179" si="140">IF(E179=0,"",$E179)</f>
+        <v/>
       </c>
       <c r="AA179" s="1" t="str">
-        <f t="shared" si="127"/>
-        <v>14.1.0</v>
+        <f t="shared" ref="AA179" si="141">IF(E179=0,"",$B179)</f>
+        <v/>
       </c>
       <c r="AC179" s="1" t="str">
         <f t="shared" si="65"/>
-        <v/>
+        <v>1.7.0</v>
       </c>
       <c r="AD179" s="1" t="str">
         <f t="shared" si="66"/>
-        <v/>
+        <v>14.1.0</v>
       </c>
       <c r="AE179" s="1" t="str">
         <f t="shared" si="67"/>
-        <v/>
+        <v>9.0.0</v>
       </c>
       <c r="AF179" s="1" t="str">
         <f t="shared" si="68"/>
-        <v/>
+        <v>10.0.0</v>
       </c>
       <c r="AG179" s="1" t="str">
         <f t="shared" si="69"/>
-        <v/>
+        <v>7.0.0</v>
       </c>
       <c r="AH179" s="1" t="str">
         <f t="shared" si="70"/>
-        <v/>
+        <v>14.1.0</v>
       </c>
       <c r="AI179" s="1" t="str">
         <f t="shared" si="71"/>
-        <v/>
+        <v>3.0.0</v>
       </c>
       <c r="AJ179" s="1" t="str">
         <f t="shared" si="72"/>
-        <v/>
+        <v>2.0.0</v>
       </c>
       <c r="AL179" s="1" t="str">
         <f t="shared" si="73"/>
-        <v>1.6.0</v>
+        <v/>
       </c>
       <c r="AM179" s="1" t="str">
         <f t="shared" si="74"/>
-        <v>14.1.0</v>
+        <v/>
       </c>
       <c r="AN179" s="1" t="str">
         <f t="shared" si="75"/>
-        <v>2.0.0</v>
+        <v/>
       </c>
       <c r="AO179" s="1" t="str">
         <f t="shared" si="76"/>
-        <v>4.0.0</v>
+        <v/>
       </c>
       <c r="AP179" s="1" t="str">
         <f t="shared" si="77"/>
-        <v>7.0.0</v>
+        <v/>
       </c>
       <c r="AQ179" s="1" t="str">
         <f t="shared" si="78"/>
-        <v>14.1.0</v>
+        <v/>
       </c>
       <c r="AR179" s="1" t="str">
         <f t="shared" si="79"/>
+        <v/>
+      </c>
+      <c r="AS179" s="1" t="str">
+        <f t="shared" si="80"/>
+        <v/>
+      </c>
+    </row>
+    <row r="180" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="str">
+        <f t="shared" ref="A180" si="142">A179</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="B180" s="3" t="str">
+        <f t="shared" si="128"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="C180" s="3"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F180" s="12"/>
+      <c r="G180" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H180" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I180" s="12"/>
+      <c r="J180" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K180" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L180" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N180" s="1" t="str">
+        <f t="shared" ref="N180" si="143">A180</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="O180" s="1" t="str">
+        <f t="shared" ref="O180" si="144">B180</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="Q180" s="1" t="str">
+        <f t="shared" ref="Q180" si="145">IF(C180=0,"",$A180)</f>
+        <v/>
+      </c>
+      <c r="R180" s="1" t="str">
+        <f t="shared" ref="R180" si="146">IF(C180=0,"",$C180)</f>
+        <v/>
+      </c>
+      <c r="S180" s="1" t="str">
+        <f t="shared" ref="S180" si="147">IF(C180=0,"",$B180)</f>
+        <v/>
+      </c>
+      <c r="U180" s="1" t="str">
+        <f t="shared" ref="U180" si="148">IF(D180=0,"",$A180)</f>
+        <v/>
+      </c>
+      <c r="V180" s="1" t="str">
+        <f t="shared" ref="V180" si="149">IF(D180=0,"",$D180)</f>
+        <v/>
+      </c>
+      <c r="W180" s="1" t="str">
+        <f t="shared" ref="W180" si="150">IF(D180=0,"",$B180)</f>
+        <v/>
+      </c>
+      <c r="Y180" s="1" t="str">
+        <f t="shared" ref="Y180" si="151">IF(E180=0,"",$A180)</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="Z180" s="1" t="str">
+        <f t="shared" ref="Z180" si="152">IF(E180=0,"",$E180)</f>
+        <v>4.0.0</v>
+      </c>
+      <c r="AA180" s="1" t="str">
+        <f t="shared" ref="AA180" si="153">IF(E180=0,"",$B180)</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="AC180" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v/>
+      </c>
+      <c r="AD180" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v/>
+      </c>
+      <c r="AE180" s="1" t="str">
+        <f t="shared" si="67"/>
+        <v/>
+      </c>
+      <c r="AF180" s="1" t="str">
+        <f t="shared" si="68"/>
+        <v/>
+      </c>
+      <c r="AG180" s="1" t="str">
+        <f t="shared" si="69"/>
+        <v/>
+      </c>
+      <c r="AH180" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v/>
+      </c>
+      <c r="AI180" s="1" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="AJ180" s="1" t="str">
+        <f t="shared" si="72"/>
+        <v/>
+      </c>
+      <c r="AL180" s="1" t="str">
+        <f t="shared" si="73"/>
+        <v>1.6.0</v>
+      </c>
+      <c r="AM180" s="1" t="str">
+        <f t="shared" si="74"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="AN180" s="1" t="str">
+        <f t="shared" si="75"/>
+        <v>2.0.0</v>
+      </c>
+      <c r="AO180" s="1" t="str">
+        <f t="shared" si="76"/>
+        <v>4.0.0</v>
+      </c>
+      <c r="AP180" s="1" t="str">
+        <f t="shared" si="77"/>
+        <v>7.0.0</v>
+      </c>
+      <c r="AQ180" s="1" t="str">
+        <f t="shared" si="78"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="AR180" s="1" t="str">
+        <f t="shared" si="79"/>
         <v>3.0.0</v>
       </c>
-      <c r="AS179" s="1" t="str">
+      <c r="AS180" s="1" t="str">
+        <f t="shared" si="80"/>
+        <v>2.0.0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="str">
+        <f t="shared" ref="A181" si="154">A180</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="B181" s="3" t="str">
+        <f t="shared" si="128"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="C181" s="3"/>
+      <c r="D181" s="12"/>
+      <c r="E181" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F181" s="12"/>
+      <c r="G181" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H181" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I181" s="12"/>
+      <c r="J181" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="K181" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L181" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N181" s="1" t="str">
+        <f t="shared" ref="N181" si="155">A181</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="O181" s="1" t="str">
+        <f t="shared" ref="O181" si="156">B181</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="Q181" s="1" t="str">
+        <f t="shared" ref="Q181" si="157">IF(C181=0,"",$A181)</f>
+        <v/>
+      </c>
+      <c r="R181" s="1" t="str">
+        <f t="shared" ref="R181" si="158">IF(C181=0,"",$C181)</f>
+        <v/>
+      </c>
+      <c r="S181" s="1" t="str">
+        <f t="shared" ref="S181" si="159">IF(C181=0,"",$B181)</f>
+        <v/>
+      </c>
+      <c r="U181" s="1" t="str">
+        <f t="shared" ref="U181" si="160">IF(D181=0,"",$A181)</f>
+        <v/>
+      </c>
+      <c r="V181" s="1" t="str">
+        <f t="shared" ref="V181" si="161">IF(D181=0,"",$D181)</f>
+        <v/>
+      </c>
+      <c r="W181" s="1" t="str">
+        <f t="shared" ref="W181" si="162">IF(D181=0,"",$B181)</f>
+        <v/>
+      </c>
+      <c r="Y181" s="1" t="str">
+        <f t="shared" ref="Y181" si="163">IF(E181=0,"",$A181)</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="Z181" s="1" t="str">
+        <f t="shared" ref="Z181" si="164">IF(E181=0,"",$E181)</f>
+        <v>4.0.0</v>
+      </c>
+      <c r="AA181" s="1" t="str">
+        <f t="shared" ref="AA181" si="165">IF(E181=0,"",$B181)</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="AC181" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v/>
+      </c>
+      <c r="AD181" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v/>
+      </c>
+      <c r="AE181" s="1" t="str">
+        <f t="shared" si="67"/>
+        <v/>
+      </c>
+      <c r="AF181" s="1" t="str">
+        <f t="shared" si="68"/>
+        <v/>
+      </c>
+      <c r="AG181" s="1" t="str">
+        <f t="shared" si="69"/>
+        <v/>
+      </c>
+      <c r="AH181" s="1" t="str">
+        <f t="shared" si="70"/>
+        <v/>
+      </c>
+      <c r="AI181" s="1" t="str">
+        <f t="shared" si="71"/>
+        <v/>
+      </c>
+      <c r="AJ181" s="1" t="str">
+        <f t="shared" si="72"/>
+        <v/>
+      </c>
+      <c r="AL181" s="1" t="str">
+        <f t="shared" si="73"/>
+        <v>1.7.0</v>
+      </c>
+      <c r="AM181" s="1" t="str">
+        <f t="shared" si="74"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="AN181" s="1" t="str">
+        <f t="shared" si="75"/>
+        <v>2.0.0</v>
+      </c>
+      <c r="AO181" s="1" t="str">
+        <f t="shared" si="76"/>
+        <v>4.0.0</v>
+      </c>
+      <c r="AP181" s="1" t="str">
+        <f t="shared" si="77"/>
+        <v>7.0.0</v>
+      </c>
+      <c r="AQ181" s="1" t="str">
+        <f t="shared" si="78"/>
+        <v>14.1.0</v>
+      </c>
+      <c r="AR181" s="1" t="str">
+        <f t="shared" si="79"/>
+        <v>3.0.0</v>
+      </c>
+      <c r="AS181" s="1" t="str">
         <f t="shared" si="80"/>
         <v>2.0.0</v>
       </c>
@@ -24956,23 +25241,23 @@
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" t="str">
         <f>tables!N180</f>
-        <v>0</v>
-      </c>
-      <c r="B45">
+        <v>14.1.0</v>
+      </c>
+      <c r="B45" t="str">
         <f>tables!O180</f>
-        <v>0</v>
+        <v>14.1.0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" t="str">
         <f>tables!N181</f>
-        <v>0</v>
-      </c>
-      <c r="B46">
+        <v>14.1.0</v>
+      </c>
+      <c r="B46" t="str">
         <f>tables!O181</f>
-        <v>0</v>
+        <v>14.1.0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -27465,31 +27750,31 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178">
+      <c r="A178" t="str">
         <f>tables!Q180</f>
-        <v>0</v>
-      </c>
-      <c r="B178">
+        <v/>
+      </c>
+      <c r="B178" t="str">
         <f>tables!R180</f>
-        <v>0</v>
-      </c>
-      <c r="C178">
+        <v/>
+      </c>
+      <c r="C178" t="str">
         <f>tables!S180</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179">
+      <c r="A179" t="str">
         <f>tables!Q181</f>
-        <v>0</v>
-      </c>
-      <c r="B179">
+        <v/>
+      </c>
+      <c r="B179" t="str">
         <f>tables!R181</f>
-        <v>0</v>
-      </c>
-      <c r="C179">
+        <v/>
+      </c>
+      <c r="C179" t="str">
         <f>tables!S181</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -30128,43 +30413,43 @@
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f>tables!U179</f>
-        <v/>
+        <v>14.1.0</v>
       </c>
       <c r="B177" t="str">
         <f>tables!V179</f>
-        <v/>
+        <v>10.0.0</v>
       </c>
       <c r="C177" t="str">
         <f>tables!W179</f>
-        <v/>
+        <v>14.1.0</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A178">
+      <c r="A178" t="str">
         <f>tables!U180</f>
-        <v>0</v>
-      </c>
-      <c r="B178">
+        <v/>
+      </c>
+      <c r="B178" t="str">
         <f>tables!V180</f>
-        <v>0</v>
-      </c>
-      <c r="C178">
+        <v/>
+      </c>
+      <c r="C178" t="str">
         <f>tables!W180</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A179">
+      <c r="A179" t="str">
         <f>tables!U181</f>
-        <v>0</v>
-      </c>
-      <c r="B179">
+        <v/>
+      </c>
+      <c r="B179" t="str">
         <f>tables!V181</f>
-        <v>0</v>
-      </c>
-      <c r="C179">
+        <v/>
+      </c>
+      <c r="C179" t="str">
         <f>tables!W181</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -30725,7 +31010,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33389,103 +33674,103 @@
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="str">
         <f>tables!AC179</f>
-        <v/>
+        <v>1.7.0</v>
       </c>
       <c r="B83" t="str">
         <f>tables!AD179</f>
-        <v/>
+        <v>14.1.0</v>
       </c>
       <c r="C83" t="str">
         <f>tables!AE179</f>
-        <v/>
+        <v>9.0.0</v>
       </c>
       <c r="D83" t="str">
         <f>tables!AF179</f>
-        <v/>
+        <v>10.0.0</v>
       </c>
       <c r="E83" t="str">
         <f>tables!AG179</f>
-        <v/>
+        <v>7.0.0</v>
       </c>
       <c r="F83" t="str">
         <f>tables!AH179</f>
-        <v/>
+        <v>14.1.0</v>
       </c>
       <c r="G83" t="str">
         <f>tables!AI179</f>
-        <v/>
+        <v>3.0.0</v>
       </c>
       <c r="H83" t="str">
         <f>tables!AJ179</f>
-        <v/>
+        <v>2.0.0</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" t="str">
         <f>tables!AC180</f>
-        <v>0</v>
-      </c>
-      <c r="B84">
+        <v/>
+      </c>
+      <c r="B84" t="str">
         <f>tables!AD180</f>
-        <v>0</v>
-      </c>
-      <c r="C84">
+        <v/>
+      </c>
+      <c r="C84" t="str">
         <f>tables!AE180</f>
-        <v>0</v>
-      </c>
-      <c r="D84">
+        <v/>
+      </c>
+      <c r="D84" t="str">
         <f>tables!AF180</f>
-        <v>0</v>
-      </c>
-      <c r="E84">
+        <v/>
+      </c>
+      <c r="E84" t="str">
         <f>tables!AG180</f>
-        <v>0</v>
-      </c>
-      <c r="F84">
+        <v/>
+      </c>
+      <c r="F84" t="str">
         <f>tables!AH180</f>
-        <v>0</v>
-      </c>
-      <c r="G84">
+        <v/>
+      </c>
+      <c r="G84" t="str">
         <f>tables!AI180</f>
-        <v>0</v>
-      </c>
-      <c r="H84">
+        <v/>
+      </c>
+      <c r="H84" t="str">
         <f>tables!AJ180</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85">
+      <c r="A85" t="str">
         <f>tables!AC181</f>
-        <v>0</v>
-      </c>
-      <c r="B85">
+        <v/>
+      </c>
+      <c r="B85" t="str">
         <f>tables!AD181</f>
-        <v>0</v>
-      </c>
-      <c r="C85">
+        <v/>
+      </c>
+      <c r="C85" t="str">
         <f>tables!AE181</f>
-        <v>0</v>
-      </c>
-      <c r="D85">
+        <v/>
+      </c>
+      <c r="D85" t="str">
         <f>tables!AF181</f>
-        <v>0</v>
-      </c>
-      <c r="E85">
+        <v/>
+      </c>
+      <c r="E85" t="str">
         <f>tables!AG181</f>
-        <v>0</v>
-      </c>
-      <c r="F85">
+        <v/>
+      </c>
+      <c r="F85" t="str">
         <f>tables!AH181</f>
-        <v>0</v>
-      </c>
-      <c r="G85">
+        <v/>
+      </c>
+      <c r="G85" t="str">
         <f>tables!AI181</f>
-        <v>0</v>
-      </c>
-      <c r="H85">
+        <v/>
+      </c>
+      <c r="H85" t="str">
         <f>tables!AJ181</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -41931,8 +42216,8 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42726,103 +43011,103 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>tables!AL179</f>
-        <v>1.6.0</v>
+        <v/>
       </c>
       <c r="B24" t="str">
         <f>tables!AM179</f>
-        <v>14.1.0</v>
+        <v/>
       </c>
       <c r="C24" t="str">
         <f>tables!AN179</f>
-        <v>2.0.0</v>
+        <v/>
       </c>
       <c r="D24" t="str">
         <f>tables!AO179</f>
-        <v>4.0.0</v>
+        <v/>
       </c>
       <c r="E24" t="str">
         <f>tables!AP179</f>
-        <v>7.0.0</v>
+        <v/>
       </c>
       <c r="F24" t="str">
         <f>tables!AQ179</f>
-        <v>14.1.0</v>
+        <v/>
       </c>
       <c r="G24" t="str">
         <f>tables!AR179</f>
-        <v>3.0.0</v>
+        <v/>
       </c>
       <c r="H24" t="str">
         <f>tables!AS179</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>tables!AL180</f>
+        <v>1.6.0</v>
+      </c>
+      <c r="B25" t="str">
+        <f>tables!AM180</f>
+        <v>14.1.0</v>
+      </c>
+      <c r="C25" t="str">
+        <f>tables!AN180</f>
         <v>2.0.0</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <f>tables!AL180</f>
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <f>tables!AM180</f>
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <f>tables!AN180</f>
-        <v>0</v>
-      </c>
-      <c r="D25">
+      <c r="D25" t="str">
         <f>tables!AO180</f>
-        <v>0</v>
-      </c>
-      <c r="E25">
+        <v>4.0.0</v>
+      </c>
+      <c r="E25" t="str">
         <f>tables!AP180</f>
-        <v>0</v>
-      </c>
-      <c r="F25">
+        <v>7.0.0</v>
+      </c>
+      <c r="F25" t="str">
         <f>tables!AQ180</f>
-        <v>0</v>
-      </c>
-      <c r="G25">
+        <v>14.1.0</v>
+      </c>
+      <c r="G25" t="str">
         <f>tables!AR180</f>
-        <v>0</v>
-      </c>
-      <c r="H25">
+        <v>3.0.0</v>
+      </c>
+      <c r="H25" t="str">
         <f>tables!AS180</f>
-        <v>0</v>
+        <v>2.0.0</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" t="str">
         <f>tables!AL181</f>
-        <v>0</v>
-      </c>
-      <c r="B26">
+        <v>1.7.0</v>
+      </c>
+      <c r="B26" t="str">
         <f>tables!AM181</f>
-        <v>0</v>
-      </c>
-      <c r="C26">
+        <v>14.1.0</v>
+      </c>
+      <c r="C26" t="str">
         <f>tables!AN181</f>
-        <v>0</v>
-      </c>
-      <c r="D26">
+        <v>2.0.0</v>
+      </c>
+      <c r="D26" t="str">
         <f>tables!AO181</f>
-        <v>0</v>
-      </c>
-      <c r="E26">
+        <v>4.0.0</v>
+      </c>
+      <c r="E26" t="str">
         <f>tables!AP181</f>
-        <v>0</v>
-      </c>
-      <c r="F26">
+        <v>7.0.0</v>
+      </c>
+      <c r="F26" t="str">
         <f>tables!AQ181</f>
-        <v>0</v>
-      </c>
-      <c r="G26">
+        <v>14.1.0</v>
+      </c>
+      <c r="G26" t="str">
         <f>tables!AR181</f>
-        <v>0</v>
-      </c>
-      <c r="H26">
+        <v>3.0.0</v>
+      </c>
+      <c r="H26" t="str">
         <f>tables!AS181</f>
-        <v>0</v>
+        <v>2.0.0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
replace 14.1.0 by 14.1.1
</commit_message>
<xml_diff>
--- a/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
+++ b/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_pub\docs\VEEPortingGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DC6B09-22D2-4673-9622-B97394F04EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C8A3FE-A452-4DC0-AB0D-AE341ACC9ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="502" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
   </bookViews>
@@ -307,13 +307,13 @@
     <t>14.0.2</t>
   </si>
   <si>
-    <t>14.1.0</t>
-  </si>
-  <si>
     <t>10.0.0</t>
   </si>
   <si>
     <t>1.7.0</t>
+  </si>
+  <si>
+    <t>14.1.1</t>
   </si>
 </sst>
 </file>
@@ -407,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +421,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -428,15 +431,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -756,32 +750,32 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" s="4" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -890,7 +884,7 @@
       <c r="J6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="7" t="s">
         <v>49</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -1033,7 +1027,7 @@
       <c r="D11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1065,7 +1059,7 @@
       <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="7" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1110,15 +1104,15 @@
       <c r="C14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="H14" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="H14" s="11" t="s">
-        <v>93</v>
-      </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="7" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="1"/>
@@ -1148,8 +1142,8 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>91</v>
+      <c r="B16" s="7" t="s">
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
@@ -1168,7 +1162,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="1"/>
@@ -1282,13 +1276,13 @@
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>91</v>
+      <c r="A26" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1308,7 +1302,7 @@
       <pane xSplit="12" ySplit="3" topLeftCell="M157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I181" sqref="I181"/>
+      <selection pane="bottomRight" activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,65 +1331,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="4"/>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="8"/>
+      <c r="O1" s="9"/>
       <c r="P1" s="6"/>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
       <c r="T1" s="6"/>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
       <c r="X1" s="6"/>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
       <c r="AB1" s="6"/>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
       <c r="AK1" s="5"/>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -23419,11 +23413,11 @@
     </row>
     <row r="172" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B172" s="3" t="str">
         <f>A172</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C172" s="3"/>
       <c r="D172" s="3"/>
@@ -23436,47 +23430,47 @@
       <c r="K172" s="3"/>
       <c r="L172" s="3"/>
       <c r="N172" s="1" t="str">
-        <f t="shared" ref="N172:N179" si="117">A172</f>
-        <v>14.1.0</v>
+        <f t="shared" ref="N172:N178" si="117">A172</f>
+        <v>14.1.1</v>
       </c>
       <c r="O172" s="1" t="str">
-        <f t="shared" ref="O172:O179" si="118">B172</f>
-        <v>14.1.0</v>
+        <f t="shared" ref="O172:O178" si="118">B172</f>
+        <v>14.1.1</v>
       </c>
       <c r="Q172" s="1" t="str">
-        <f t="shared" ref="Q172:Q179" si="119">IF(C172=0,"",$A172)</f>
+        <f t="shared" ref="Q172:Q178" si="119">IF(C172=0,"",$A172)</f>
         <v/>
       </c>
       <c r="R172" s="1" t="str">
-        <f t="shared" ref="R172:R179" si="120">IF(C172=0,"",$C172)</f>
+        <f t="shared" ref="R172:R178" si="120">IF(C172=0,"",$C172)</f>
         <v/>
       </c>
       <c r="S172" s="1" t="str">
-        <f t="shared" ref="S172:S179" si="121">IF(C172=0,"",$B172)</f>
+        <f t="shared" ref="S172:S178" si="121">IF(C172=0,"",$B172)</f>
         <v/>
       </c>
       <c r="U172" s="1" t="str">
-        <f t="shared" ref="U172:U179" si="122">IF(D172=0,"",$A172)</f>
+        <f t="shared" ref="U172:U178" si="122">IF(D172=0,"",$A172)</f>
         <v/>
       </c>
       <c r="V172" s="1" t="str">
-        <f t="shared" ref="V172:V179" si="123">IF(D172=0,"",$D172)</f>
+        <f t="shared" ref="V172:V178" si="123">IF(D172=0,"",$D172)</f>
         <v/>
       </c>
       <c r="W172" s="1" t="str">
-        <f t="shared" ref="W172:W179" si="124">IF(D172=0,"",$B172)</f>
+        <f t="shared" ref="W172:W178" si="124">IF(D172=0,"",$B172)</f>
         <v/>
       </c>
       <c r="Y172" s="1" t="str">
-        <f t="shared" ref="Y172:Y179" si="125">IF(E172=0,"",$A172)</f>
+        <f t="shared" ref="Y172:Y178" si="125">IF(E172=0,"",$A172)</f>
         <v/>
       </c>
       <c r="Z172" s="1" t="str">
-        <f t="shared" ref="Z172:Z179" si="126">IF(E172=0,"",$E172)</f>
+        <f t="shared" ref="Z172:Z178" si="126">IF(E172=0,"",$E172)</f>
         <v/>
       </c>
       <c r="AA172" s="1" t="str">
-        <f t="shared" ref="AA172:AA179" si="127">IF(E172=0,"",$B172)</f>
+        <f t="shared" ref="AA172:AA178" si="127">IF(E172=0,"",$B172)</f>
         <v/>
       </c>
       <c r="AC172" s="1" t="str">
@@ -23547,11 +23541,11 @@
     <row r="173" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="str">
         <f>A172</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B173" s="3" t="str">
         <f t="shared" ref="B173:B181" si="128">A173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C173" s="3" t="s">
         <v>3</v>
@@ -23567,15 +23561,15 @@
       <c r="L173" s="3"/>
       <c r="N173" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O173" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q173" s="1" t="str">
         <f t="shared" si="119"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="R173" s="1" t="str">
         <f t="shared" si="120"/>
@@ -23583,7 +23577,7 @@
       </c>
       <c r="S173" s="1" t="str">
         <f t="shared" si="121"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="U173" s="1" t="str">
         <f t="shared" si="122"/>
@@ -23677,15 +23671,15 @@
     <row r="174" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="str">
         <f t="shared" ref="A174:A178" si="129">A173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B174" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E174" s="3"/>
       <c r="F174" s="3"/>
@@ -23697,11 +23691,11 @@
       <c r="L174" s="3"/>
       <c r="N174" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O174" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q174" s="1" t="str">
         <f t="shared" si="119"/>
@@ -23717,7 +23711,7 @@
       </c>
       <c r="U174" s="1" t="str">
         <f t="shared" si="122"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="V174" s="1" t="str">
         <f t="shared" si="123"/>
@@ -23725,7 +23719,7 @@
       </c>
       <c r="W174" s="1" t="str">
         <f t="shared" si="124"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Y174" s="1" t="str">
         <f t="shared" si="125"/>
@@ -23807,11 +23801,11 @@
     <row r="175" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="str">
         <f t="shared" si="129"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B175" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C175" s="3"/>
       <c r="D175" s="3"/>
@@ -23827,11 +23821,11 @@
       <c r="L175" s="3"/>
       <c r="N175" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O175" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q175" s="1" t="str">
         <f t="shared" si="119"/>
@@ -23859,7 +23853,7 @@
       </c>
       <c r="Y175" s="1" t="str">
         <f t="shared" si="125"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Z175" s="1" t="str">
         <f t="shared" si="126"/>
@@ -23867,7 +23861,7 @@
       </c>
       <c r="AA175" s="1" t="str">
         <f t="shared" si="127"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AC175" s="1" t="str">
         <f t="shared" si="65"/>
@@ -23937,41 +23931,41 @@
     <row r="176" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="str">
         <f t="shared" si="129"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B176" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C176" s="3"/>
-      <c r="D176" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E176" s="12"/>
-      <c r="F176" s="12"/>
-      <c r="G176" s="12" t="s">
+      <c r="D176" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E176" s="3"/>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H176" s="12" t="s">
+      <c r="H176" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I176" s="12" t="s">
+      <c r="I176" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J176" s="12"/>
-      <c r="K176" s="12" t="s">
+      <c r="J176" s="3"/>
+      <c r="K176" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L176" s="12" t="s">
+      <c r="L176" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N176" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O176" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q176" s="1" t="str">
         <f t="shared" si="119"/>
@@ -23987,7 +23981,7 @@
       </c>
       <c r="U176" s="1" t="str">
         <f t="shared" si="122"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="V176" s="1" t="str">
         <f t="shared" si="123"/>
@@ -23995,7 +23989,7 @@
       </c>
       <c r="W176" s="1" t="str">
         <f t="shared" si="124"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Y176" s="1" t="str">
         <f t="shared" si="125"/>
@@ -24015,7 +24009,7 @@
       </c>
       <c r="AD176" s="1" t="str">
         <f t="shared" si="66"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AE176" s="1" t="str">
         <f t="shared" si="67"/>
@@ -24031,7 +24025,7 @@
       </c>
       <c r="AH176" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AI176" s="1" t="str">
         <f t="shared" si="71"/>
@@ -24077,41 +24071,41 @@
     <row r="177" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="str">
         <f t="shared" si="129"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B177" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C177" s="3"/>
-      <c r="D177" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E177" s="12"/>
-      <c r="F177" s="12"/>
-      <c r="G177" s="12" t="s">
+      <c r="D177" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E177" s="3"/>
+      <c r="F177" s="3"/>
+      <c r="G177" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H177" s="12" t="s">
+      <c r="H177" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I177" s="12" t="s">
+      <c r="I177" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J177" s="12"/>
-      <c r="K177" s="12" t="s">
+      <c r="J177" s="3"/>
+      <c r="K177" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L177" s="12" t="s">
+      <c r="L177" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N177" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O177" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q177" s="1" t="str">
         <f t="shared" si="119"/>
@@ -24127,7 +24121,7 @@
       </c>
       <c r="U177" s="1" t="str">
         <f t="shared" si="122"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="V177" s="1" t="str">
         <f t="shared" si="123"/>
@@ -24135,7 +24129,7 @@
       </c>
       <c r="W177" s="1" t="str">
         <f t="shared" si="124"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Y177" s="1" t="str">
         <f t="shared" si="125"/>
@@ -24155,7 +24149,7 @@
       </c>
       <c r="AD177" s="1" t="str">
         <f t="shared" si="66"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AE177" s="1" t="str">
         <f t="shared" si="67"/>
@@ -24171,7 +24165,7 @@
       </c>
       <c r="AH177" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AI177" s="1" t="str">
         <f t="shared" si="71"/>
@@ -24217,41 +24211,41 @@
     <row r="178" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="str">
         <f t="shared" si="129"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B178" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C178" s="3"/>
-      <c r="D178" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E178" s="12"/>
-      <c r="F178" s="12"/>
-      <c r="G178" s="12" t="s">
+      <c r="D178" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E178" s="3"/>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H178" s="12" t="s">
+      <c r="H178" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I178" s="12" t="s">
+      <c r="I178" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J178" s="12"/>
-      <c r="K178" s="12" t="s">
+      <c r="J178" s="3"/>
+      <c r="K178" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L178" s="12" t="s">
+      <c r="L178" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N178" s="1" t="str">
         <f t="shared" si="117"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O178" s="1" t="str">
         <f t="shared" si="118"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q178" s="1" t="str">
         <f t="shared" si="119"/>
@@ -24267,7 +24261,7 @@
       </c>
       <c r="U178" s="1" t="str">
         <f t="shared" si="122"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="V178" s="1" t="str">
         <f t="shared" si="123"/>
@@ -24275,7 +24269,7 @@
       </c>
       <c r="W178" s="1" t="str">
         <f t="shared" si="124"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Y178" s="1" t="str">
         <f t="shared" si="125"/>
@@ -24295,7 +24289,7 @@
       </c>
       <c r="AD178" s="1" t="str">
         <f t="shared" si="66"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AE178" s="1" t="str">
         <f t="shared" si="67"/>
@@ -24311,7 +24305,7 @@
       </c>
       <c r="AH178" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AI178" s="1" t="str">
         <f t="shared" si="71"/>
@@ -24357,41 +24351,41 @@
     <row r="179" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="str">
         <f t="shared" ref="A179" si="130">A178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B179" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C179" s="3"/>
-      <c r="D179" s="12" t="s">
+      <c r="D179" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E179" s="12"/>
-      <c r="F179" s="12"/>
-      <c r="G179" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H179" s="12" t="s">
+      <c r="H179" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I179" s="12" t="s">
+      <c r="I179" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J179" s="12"/>
-      <c r="K179" s="12" t="s">
+      <c r="J179" s="3"/>
+      <c r="K179" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L179" s="12" t="s">
+      <c r="L179" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N179" s="1" t="str">
         <f t="shared" ref="N179" si="131">A179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O179" s="1" t="str">
         <f t="shared" ref="O179" si="132">B179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q179" s="1" t="str">
         <f t="shared" ref="Q179" si="133">IF(C179=0,"",$A179)</f>
@@ -24407,7 +24401,7 @@
       </c>
       <c r="U179" s="1" t="str">
         <f t="shared" ref="U179" si="136">IF(D179=0,"",$A179)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="V179" s="1" t="str">
         <f t="shared" ref="V179" si="137">IF(D179=0,"",$D179)</f>
@@ -24415,7 +24409,7 @@
       </c>
       <c r="W179" s="1" t="str">
         <f t="shared" ref="W179" si="138">IF(D179=0,"",$B179)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Y179" s="1" t="str">
         <f t="shared" ref="Y179" si="139">IF(E179=0,"",$A179)</f>
@@ -24435,7 +24429,7 @@
       </c>
       <c r="AD179" s="1" t="str">
         <f t="shared" si="66"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AE179" s="1" t="str">
         <f t="shared" si="67"/>
@@ -24451,7 +24445,7 @@
       </c>
       <c r="AH179" s="1" t="str">
         <f t="shared" si="70"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AI179" s="1" t="str">
         <f t="shared" si="71"/>
@@ -24497,41 +24491,41 @@
     <row r="180" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="str">
         <f t="shared" ref="A180" si="142">A179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B180" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C180" s="3"/>
-      <c r="D180" s="12"/>
-      <c r="E180" s="12" t="s">
+      <c r="D180" s="3"/>
+      <c r="E180" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F180" s="12"/>
-      <c r="G180" s="12" t="s">
+      <c r="F180" s="3"/>
+      <c r="G180" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H180" s="12" t="s">
+      <c r="H180" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I180" s="12"/>
-      <c r="J180" s="12" t="s">
+      <c r="I180" s="3"/>
+      <c r="J180" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K180" s="12" t="s">
+      <c r="K180" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L180" s="12" t="s">
+      <c r="L180" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N180" s="1" t="str">
         <f t="shared" ref="N180" si="143">A180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O180" s="1" t="str">
         <f t="shared" ref="O180" si="144">B180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q180" s="1" t="str">
         <f t="shared" ref="Q180" si="145">IF(C180=0,"",$A180)</f>
@@ -24559,7 +24553,7 @@
       </c>
       <c r="Y180" s="1" t="str">
         <f t="shared" ref="Y180" si="151">IF(E180=0,"",$A180)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Z180" s="1" t="str">
         <f t="shared" ref="Z180" si="152">IF(E180=0,"",$E180)</f>
@@ -24567,7 +24561,7 @@
       </c>
       <c r="AA180" s="1" t="str">
         <f t="shared" ref="AA180" si="153">IF(E180=0,"",$B180)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AC180" s="1" t="str">
         <f t="shared" si="65"/>
@@ -24607,7 +24601,7 @@
       </c>
       <c r="AM180" s="1" t="str">
         <f t="shared" si="74"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AN180" s="1" t="str">
         <f t="shared" si="75"/>
@@ -24623,7 +24617,7 @@
       </c>
       <c r="AQ180" s="1" t="str">
         <f t="shared" si="78"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AR180" s="1" t="str">
         <f t="shared" si="79"/>
@@ -24637,41 +24631,41 @@
     <row r="181" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="str">
         <f t="shared" ref="A181" si="154">A180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B181" s="3" t="str">
         <f t="shared" si="128"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C181" s="3"/>
-      <c r="D181" s="12"/>
-      <c r="E181" s="12" t="s">
+      <c r="D181" s="3"/>
+      <c r="E181" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F181" s="12"/>
-      <c r="G181" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="H181" s="12" t="s">
+      <c r="F181" s="3"/>
+      <c r="G181" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H181" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I181" s="12"/>
-      <c r="J181" s="12" t="s">
+      <c r="I181" s="3"/>
+      <c r="J181" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="K181" s="12" t="s">
+      <c r="K181" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="L181" s="12" t="s">
+      <c r="L181" s="3" t="s">
         <v>49</v>
       </c>
       <c r="N181" s="1" t="str">
         <f t="shared" ref="N181" si="155">A181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="O181" s="1" t="str">
         <f t="shared" ref="O181" si="156">B181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Q181" s="1" t="str">
         <f t="shared" ref="Q181" si="157">IF(C181=0,"",$A181)</f>
@@ -24699,7 +24693,7 @@
       </c>
       <c r="Y181" s="1" t="str">
         <f t="shared" ref="Y181" si="163">IF(E181=0,"",$A181)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="Z181" s="1" t="str">
         <f t="shared" ref="Z181" si="164">IF(E181=0,"",$E181)</f>
@@ -24707,7 +24701,7 @@
       </c>
       <c r="AA181" s="1" t="str">
         <f t="shared" ref="AA181" si="165">IF(E181=0,"",$B181)</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AC181" s="1" t="str">
         <f t="shared" si="65"/>
@@ -24747,7 +24741,7 @@
       </c>
       <c r="AM181" s="1" t="str">
         <f t="shared" si="74"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AN181" s="1" t="str">
         <f t="shared" si="75"/>
@@ -24763,7 +24757,7 @@
       </c>
       <c r="AQ181" s="1" t="str">
         <f t="shared" si="78"/>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="AR181" s="1" t="str">
         <f t="shared" si="79"/>
@@ -25163,101 +25157,101 @@
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>tables!N172</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B37" t="str">
         <f>tables!O172</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>tables!N173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B38" t="str">
         <f>tables!O173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>tables!N174</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B39" t="str">
         <f>tables!O174</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>tables!N175</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B40" t="str">
         <f>tables!O175</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>tables!N176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B41" t="str">
         <f>tables!O176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>tables!N177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B42" t="str">
         <f>tables!O177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>tables!N178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B43" t="str">
         <f>tables!O178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>tables!N179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B44" t="str">
         <f>tables!O179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>tables!N180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B45" t="str">
         <f>tables!O180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>tables!N181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B46" t="str">
         <f>tables!O181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -27654,7 +27648,7 @@
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="str">
         <f>tables!Q173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B171" t="str">
         <f>tables!R173</f>
@@ -27662,7 +27656,7 @@
       </c>
       <c r="C171" t="str">
         <f>tables!S173</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -30343,7 +30337,7 @@
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="str">
         <f>tables!U174</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B172" t="str">
         <f>tables!V174</f>
@@ -30351,7 +30345,7 @@
       </c>
       <c r="C172" t="str">
         <f>tables!W174</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -30371,7 +30365,7 @@
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="str">
         <f>tables!U176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B174" t="str">
         <f>tables!V176</f>
@@ -30379,13 +30373,13 @@
       </c>
       <c r="C174" t="str">
         <f>tables!W176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="str">
         <f>tables!U177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B175" t="str">
         <f>tables!V177</f>
@@ -30393,13 +30387,13 @@
       </c>
       <c r="C175" t="str">
         <f>tables!W177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="str">
         <f>tables!U178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B176" t="str">
         <f>tables!V178</f>
@@ -30407,13 +30401,13 @@
       </c>
       <c r="C176" t="str">
         <f>tables!W178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="str">
         <f>tables!U179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B177" t="str">
         <f>tables!V179</f>
@@ -30421,7 +30415,7 @@
       </c>
       <c r="C177" t="str">
         <f>tables!W179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -30974,7 +30968,7 @@
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>tables!Y175</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="B33" t="str">
         <f>tables!Z175</f>
@@ -30982,7 +30976,7 @@
       </c>
       <c r="C33" t="str">
         <f>tables!AA175</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -33202,7 +33196,7 @@
       </c>
       <c r="B69" t="str">
         <f>tables!AD176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C69" t="str">
         <f>tables!AE176</f>
@@ -33218,7 +33212,7 @@
       </c>
       <c r="F69" t="str">
         <f>tables!AH176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G69" t="str">
         <f>tables!AI176</f>
@@ -33236,7 +33230,7 @@
       </c>
       <c r="B70" t="str">
         <f>tables!AD177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C70" t="str">
         <f>tables!AE177</f>
@@ -33252,7 +33246,7 @@
       </c>
       <c r="F70" t="str">
         <f>tables!AH177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G70" t="str">
         <f>tables!AI177</f>
@@ -33576,7 +33570,7 @@
       </c>
       <c r="B80" t="str">
         <f>tables!AD176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C80" t="str">
         <f>tables!AE176</f>
@@ -33592,7 +33586,7 @@
       </c>
       <c r="F80" t="str">
         <f>tables!AH176</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G80" t="str">
         <f>tables!AI176</f>
@@ -33610,7 +33604,7 @@
       </c>
       <c r="B81" t="str">
         <f>tables!AD177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C81" t="str">
         <f>tables!AE177</f>
@@ -33626,7 +33620,7 @@
       </c>
       <c r="F81" t="str">
         <f>tables!AH177</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G81" t="str">
         <f>tables!AI177</f>
@@ -33644,7 +33638,7 @@
       </c>
       <c r="B82" t="str">
         <f>tables!AD178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C82" t="str">
         <f>tables!AE178</f>
@@ -33660,7 +33654,7 @@
       </c>
       <c r="F82" t="str">
         <f>tables!AH178</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G82" t="str">
         <f>tables!AI178</f>
@@ -33678,7 +33672,7 @@
       </c>
       <c r="B83" t="str">
         <f>tables!AD179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C83" t="str">
         <f>tables!AE179</f>
@@ -33694,7 +33688,7 @@
       </c>
       <c r="F83" t="str">
         <f>tables!AH179</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G83" t="str">
         <f>tables!AI179</f>
@@ -43049,7 +43043,7 @@
       </c>
       <c r="B25" t="str">
         <f>tables!AM180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C25" t="str">
         <f>tables!AN180</f>
@@ -43065,7 +43059,7 @@
       </c>
       <c r="F25" t="str">
         <f>tables!AQ180</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G25" t="str">
         <f>tables!AR180</f>
@@ -43083,7 +43077,7 @@
       </c>
       <c r="B26" t="str">
         <f>tables!AM181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="C26" t="str">
         <f>tables!AN181</f>
@@ -43099,7 +43093,7 @@
       </c>
       <c r="F26" t="str">
         <f>tables!AQ181</f>
-        <v>14.1.0</v>
+        <v>14.1.1</v>
       </c>
       <c r="G26" t="str">
         <f>tables!AR181</f>

</xml_diff>

<commit_message>
review the table of testsuite UI
</commit_message>
<xml_diff>
--- a/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
+++ b/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_pub\docs\VEEPortingGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C107D32-B89C-4F0A-A2C1-0BBDF7169999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FB513E-2983-4377-9CBA-DF7838CC213B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="502" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="502" activeTab="1" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="versions" sheetId="6" r:id="rId1"/>
-    <sheet name="tables" sheetId="5" r:id="rId2"/>
-    <sheet name="ui base" sheetId="7" r:id="rId3"/>
-    <sheet name="ui dma2d" sheetId="8" r:id="rId4"/>
-    <sheet name="ui vglite" sheetId="9" r:id="rId5"/>
-    <sheet name="ui nema" sheetId="10" r:id="rId6"/>
-    <sheet name="vg vglite" sheetId="11" r:id="rId7"/>
-    <sheet name="vg_nema" sheetId="12" r:id="rId8"/>
+    <sheet name="dates" sheetId="13" r:id="rId2"/>
+    <sheet name="tables" sheetId="5" r:id="rId3"/>
+    <sheet name="ui base" sheetId="7" r:id="rId4"/>
+    <sheet name="ui dma2d" sheetId="8" r:id="rId5"/>
+    <sheet name="ui vglite" sheetId="9" r:id="rId6"/>
+    <sheet name="ui nema" sheetId="10" r:id="rId7"/>
+    <sheet name="vg vglite" sheetId="11" r:id="rId8"/>
+    <sheet name="vg_nema" sheetId="12" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="132">
   <si>
     <t>pack ui</t>
   </si>
@@ -336,12 +337,105 @@
   <si>
     <t>9.0.1</t>
   </si>
+  <si>
+    <t>MUI API</t>
+  </si>
+  <si>
+    <t>3.0.3</t>
+  </si>
+  <si>
+    <t>3.0.4</t>
+  </si>
+  <si>
+    <t>3.2.0</t>
+  </si>
+  <si>
+    <t>3.3.0</t>
+  </si>
+  <si>
+    <t>3.4.0</t>
+  </si>
+  <si>
+    <t>3.4.1</t>
+  </si>
+  <si>
+    <t>3.5.0</t>
+  </si>
+  <si>
+    <t>3.6.0</t>
+  </si>
+  <si>
+    <t>3.6.1</t>
+  </si>
+  <si>
+    <t>Drawing API</t>
+  </si>
+  <si>
+    <t>1.0.4</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>1.0.5</t>
+  </si>
+  <si>
+    <t>XPFP</t>
+  </si>
+  <si>
+    <t>13.0.5</t>
+  </si>
+  <si>
+    <t>13.4.0</t>
+  </si>
+  <si>
+    <t>13.5.0</t>
+  </si>
+  <si>
+    <t>13.7.1</t>
+  </si>
+  <si>
+    <t>14.0.3</t>
+  </si>
+  <si>
+    <t>14.1.0</t>
+  </si>
+  <si>
+    <t>14.3.1</t>
+  </si>
+  <si>
+    <t>14.4.0</t>
+  </si>
+  <si>
+    <t>14.4.2</t>
+  </si>
+  <si>
+    <t>14.5.0</t>
+  </si>
+  <si>
+    <t>14.5.1</t>
+  </si>
+  <si>
+    <t>gray = not published</t>
+  </si>
+  <si>
+    <t>Testsuite</t>
+  </si>
+  <si>
+    <t>1.8.0</t>
+  </si>
+  <si>
+    <t>1.8.1</t>
+  </si>
+  <si>
+    <t>1.8.2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +473,19 @@
     <font>
       <sz val="16"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -428,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -454,7 +561,16 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -773,7 +889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD77347-2714-4209-BB1E-7F53155AAE39}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +1024,7 @@
       <c r="J6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="1" t="s">
         <v>49</v>
       </c>
       <c r="L6" s="1" t="s">
@@ -982,7 +1098,7 @@
       <c r="J8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
@@ -1089,7 +1205,7 @@
       <c r="H12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J12" s="1" t="s">
@@ -1140,11 +1256,11 @@
         <v>91</v>
       </c>
       <c r="E14" s="1"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="1" t="s">
         <v>92</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="K14" s="1"/>
@@ -1178,7 +1294,7 @@
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="1" t="s">
         <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -1327,7 +1443,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="1" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1366,6 +1482,555 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BAB6E8-CF35-42E8-95F4-079D47989D2F}">
+  <dimension ref="A1:F53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="A4:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>44040</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>44042</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>44095</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>44096</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>44106</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>44168</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>44174</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>44211</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>44263</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>44266</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>44284</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>44393</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>44407</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>44411</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>44679</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>44686</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>44805</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>44806</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>44813</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>44911</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>44915</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>44963</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>45049</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>45085</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>45124</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>45133</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>45189</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>45222</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
+        <v>45260</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>45336</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>45281</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
+        <v>45336</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>45391</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>45393</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
+        <v>45496</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>45499</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>45566</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>45574</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
+        <v>45582</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
+        <v>45614</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
+        <v>45681</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>45688</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>45698</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
+        <v>45706</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>45723</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>45729</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
+        <v>45797</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
+        <v>45937</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>45943</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E750B59-6D36-4DC3-86F9-7C4DB63A361C}">
   <dimension ref="A1:AS243"/>
   <sheetViews>
@@ -33320,7 +33985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D3E1B2-6FBF-4321-9BDB-6B5B6C1895EC}">
   <dimension ref="A1:B106"/>
   <sheetViews>
@@ -34395,7 +35060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9A5018-D296-4BB9-8948-2B005C0B076A}">
   <dimension ref="A1:C238"/>
   <sheetViews>
@@ -37728,7 +38393,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C15CE05B-5288-4DE8-B4AC-D3F699DE2D90}">
   <dimension ref="A1:C237"/>
   <sheetViews>
@@ -41061,7 +41726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448541E8-651D-4D8E-9727-B163A1E311B1}">
   <dimension ref="A1:C95"/>
   <sheetViews>
@@ -42406,7 +43071,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43404E6D-24D5-44E7-9062-EC44A7F899D1}">
   <dimension ref="A1:I144"/>
   <sheetViews>
@@ -47187,7 +47852,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B13E2A-7960-422C-B8B4-D7E8048331C7}">
   <dimension ref="A1:I87"/>
   <sheetViews>

</xml_diff>

<commit_message>
add the table of testsuite VG
</commit_message>
<xml_diff>
--- a/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
+++ b/VEEPortingGuide/ui_vg_releases_notes_cco.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_pub\docs\VEEPortingGuide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FB513E-2983-4377-9CBA-DF7838CC213B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D9C2C7-F0B2-4C25-A5C3-BF3190A4B22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="502" activeTab="1" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="502" activeTab="1" xr2:uid="{62F6EEB7-C17F-40C9-8050-F3352CC93ED9}"/>
   </bookViews>
   <sheets>
     <sheet name="versions" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="144">
   <si>
     <t>pack ui</t>
   </si>
@@ -416,6 +416,12 @@
     <t>14.5.1</t>
   </si>
   <si>
+    <t>1.5.2</t>
+  </si>
+  <si>
+    <t>1.1.2</t>
+  </si>
+  <si>
     <t>gray = not published</t>
   </si>
   <si>
@@ -429,6 +435,36 @@
   </si>
   <si>
     <t>1.8.2</t>
+  </si>
+  <si>
+    <t>MVG API</t>
+  </si>
+  <si>
+    <t>Pack</t>
+  </si>
+  <si>
+    <t>1.7.2</t>
+  </si>
+  <si>
+    <t>2.2.0</t>
+  </si>
+  <si>
+    <t>2.3.0</t>
+  </si>
+  <si>
+    <t>2.4.0</t>
+  </si>
+  <si>
+    <t>2.5.0</t>
+  </si>
+  <si>
+    <t>2.6.0</t>
+  </si>
+  <si>
+    <t>2.7.0</t>
+  </si>
+  <si>
+    <t>4.2.0</t>
   </si>
 </sst>
 </file>
@@ -491,7 +527,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,6 +558,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -535,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -571,6 +613,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1483,13 +1531,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BAB6E8-CF35-42E8-95F4-079D47989D2F}">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="A4:E21"/>
+      <selection pane="bottomRight" activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,19 +1546,19 @@
     <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" style="15" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>101</v>
       </c>
@@ -1521,10 +1569,19 @@
         <v>115</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>44040</v>
       </c>
@@ -1535,7 +1592,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>44042</v>
       </c>
@@ -1543,7 +1600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>44095</v>
       </c>
@@ -1551,7 +1608,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>44096</v>
       </c>
@@ -1559,7 +1616,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>44106</v>
       </c>
@@ -1567,7 +1624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>44168</v>
       </c>
@@ -1581,7 +1638,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>44174</v>
       </c>
@@ -1592,7 +1649,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>44211</v>
       </c>
@@ -1600,7 +1657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>44263</v>
       </c>
@@ -1608,7 +1665,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>44266</v>
       </c>
@@ -1616,7 +1673,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>44284</v>
       </c>
@@ -1624,7 +1681,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>44393</v>
       </c>
@@ -1635,7 +1692,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>44407</v>
       </c>
@@ -1643,7 +1700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>44411</v>
       </c>
@@ -1651,7 +1708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>44679</v>
       </c>
@@ -1662,7 +1719,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>44686</v>
       </c>
@@ -1670,357 +1727,569 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
+        <v>44694</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>44697</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
         <v>44805</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
         <v>44806</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D24" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="G24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>44809</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
         <v>44813</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>44818</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
         <v>44911</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E28" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
         <v>44915</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D29" s="13" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="G29" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>44924</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="I30" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>44925</v>
+      </c>
+      <c r="D31" s="13"/>
+      <c r="H31" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>44963</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D32" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
+      <c r="H32" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>45049</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D33" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="11"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="F33" s="16"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
+        <v>45056</v>
+      </c>
+      <c r="D34" s="13"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
         <v>45085</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F28" s="11"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="11">
         <v>45124</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>45128</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>45133</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D38" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
         <v>45189</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>45190</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
         <v>45222</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E41" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="11">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>45243</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="11">
         <v>45260</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D43" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E43" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="11">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="11">
         <v>45336</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="11">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="11">
         <v>45281</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="11">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
         <v>45336</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="11">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="11">
+        <v>45337</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="11">
         <v>45391</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E37" s="13" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+      <c r="E48" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
         <v>45393</v>
       </c>
-      <c r="E38" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="11">
+      <c r="E49" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="11">
+        <v>45492</v>
+      </c>
+      <c r="E50" s="14"/>
+      <c r="H50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="11">
         <v>45496</v>
       </c>
-      <c r="E39" s="13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="11">
+      <c r="E51" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="11">
         <v>45499</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E40" s="13"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11">
+      <c r="E52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
         <v>45566</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D53" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E53" s="13" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="11">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="11">
         <v>45574</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B54" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E54" s="13" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="11">
+      <c r="G54" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="11">
         <v>45582</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D55" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E55" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="11">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
         <v>45614</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="11">
         <v>45681</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D57" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="11">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="11">
         <v>45688</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D58" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E58" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="11">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="11">
+        <v>45691</v>
+      </c>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="G59" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="11">
         <v>45698</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="11">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="11">
         <v>45706</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D61" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E61" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="11">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="11">
         <v>45723</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D62" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E62" s="13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="11">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="11">
         <v>45729</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D63" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="11">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="11">
+        <v>45756</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="11">
         <v>45797</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D65" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="11">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="11">
+        <v>45915</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="11">
+        <v>45916</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="11">
         <v>45937</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D68" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E68" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="11">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="11">
         <v>45943</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D69" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E53" s="1" t="s">
+      <c r="E69" s="1" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>